<commit_message>
fixed the calling of functions
</commit_message>
<xml_diff>
--- a/pythonProject/Results_2/Results_Accuracy_Precision.xlsx
+++ b/pythonProject/Results_2/Results_Accuracy_Precision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\MSc\Masters Project 2023\Masters-Project-2023\pythonProject\Results_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D318925F-266E-47B0-A1D5-CA003D8F2435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C638489E-6CE1-479D-93D0-8E990D5CE4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5CA8B72F-33E3-4768-B596-8D0AAD542442}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000000%"/>
+    <numFmt numFmtId="164" formatCode="0.00000000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -119,7 +119,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E089F8E1-69D8-4482-BC20-D4FBEC0203E1}">
   <dimension ref="A1:G318"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+      <selection activeCell="B287" sqref="B287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5654,18 +5654,15 @@
         <v>302</v>
       </c>
       <c r="B298">
-        <v>14</v>
-      </c>
-      <c r="C298">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F298">
         <f t="shared" si="8"/>
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="G298">
         <f t="shared" si="9"/>
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.3">
@@ -6002,11 +5999,11 @@
       </c>
       <c r="F318" s="2">
         <f>(AVERAGE(F2:F317))</f>
-        <v>0.96164804341228405</v>
+        <v>0.96204361303253716</v>
       </c>
       <c r="G318" s="2">
         <f>(AVERAGE(G2:G317))</f>
-        <v>0.96075367143405122</v>
+        <v>0.96114924105430433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving files into excel
</commit_message>
<xml_diff>
--- a/pythonProject/Results_2/Results_Accuracy_Precision.xlsx
+++ b/pythonProject/Results_2/Results_Accuracy_Precision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\MSc\Masters Project 2023\Masters-Project-2023\pythonProject\Results_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B06F98-0E01-444C-9AD6-79B3C4E9E530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF82A930-6ADD-46C9-89A7-24837435A2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5CA8B72F-33E3-4768-B596-8D0AAD542442}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>No.</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Using Distance</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -6030,35 +6033,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26CD9F93-0E95-4EDE-811A-9650DA95C7EC}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1007.8392997384</v>
+      </c>
+      <c r="D2">
+        <v>2.9599759727716401E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing elapsed time for prep
</commit_message>
<xml_diff>
--- a/pythonProject/Results_2/Results_Accuracy_Precision.xlsx
+++ b/pythonProject/Results_2/Results_Accuracy_Precision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\MSc\Masters Project 2023\Masters-Project-2023\pythonProject\Results_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF82A930-6ADD-46C9-89A7-24837435A2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06AD4DA-2173-47B8-BE81-C3F535226C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5CA8B72F-33E3-4768-B596-8D0AAD542442}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5CA8B72F-33E3-4768-B596-8D0AAD542442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>No.</t>
   </si>
@@ -61,21 +61,6 @@
   </si>
   <si>
     <t>Average</t>
-  </si>
-  <si>
-    <t>Initial Preparation Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only Single Line </t>
-  </si>
-  <si>
-    <t>Using Size</t>
-  </si>
-  <si>
-    <t>Using Distance</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -453,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E089F8E1-69D8-4482-BC20-D4FBEC0203E1}">
   <dimension ref="A1:G318"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="L301" sqref="L301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6033,10 +6018,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26CD9F93-0E95-4EDE-811A-9650DA95C7EC}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="A1:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6046,87 +6031,7 @@
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1007.8392997384</v>
-      </c>
-      <c r="D2">
-        <v>2.9599759727716401E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>